<commit_message>
Busqueda en Wikipedia por datos Excel
</commit_message>
<xml_diff>
--- a/Automation.Data/Resources/Busquedas.xlsx
+++ b/Automation.Data/Resources/Busquedas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@Source\TestAutomations\Test.Automation-CpSat\Automation.Data\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Descripcion</t>
   </si>
@@ -32,19 +32,22 @@
     <t>PrimerResultado</t>
   </si>
   <si>
-    <t>hola</t>
-  </si>
-  <si>
-    <t>mundo</t>
-  </si>
-  <si>
-    <t>hugo</t>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Driver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,7 +372,7 @@
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,23 +380,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>